<commit_message>
take out of range metric out of title in excel sheet
</commit_message>
<xml_diff>
--- a/routing_project2/Simulations.xlsx
+++ b/routing_project2/Simulations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jokubas/Desktop/ADHSN/ahsn_groupjj/routing_project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffrey/Documents/TUDelft/Assignments/MY2Q1/AHSN/ahsn_groupjj/routing_project2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C997D8E-EB1B-E848-97A9-3B607E19C716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B352199-F867-F449-A3DA-DB93E41D3A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="1680" windowWidth="27640" windowHeight="16940" xr2:uid="{5B0FB570-53D5-CC45-9C8C-CFBFA881E8D1}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="208">
   <si>
     <t>Movement</t>
   </si>
@@ -149,18 +149,12 @@
     <t xml:space="preserve"> 2.2</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 7</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.14285714285714285</t>
   </si>
   <si>
     <t xml:space="preserve"> 3.1</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 20</t>
-  </si>
-  <si>
     <t>Neighbour got out of range. 30</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t xml:space="preserve"> 3.7</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 6</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.3</t>
   </si>
   <si>
@@ -188,12 +179,6 @@
     <t xml:space="preserve"> 2.0</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 33</t>
-  </si>
-  <si>
-    <t>Neighbour got out of range. 12</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.5</t>
   </si>
   <si>
@@ -218,18 +203,12 @@
     <t xml:space="preserve"> 90.0</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 5</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.027683019638061523</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.0023069183031717935</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 13</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.1111111111111111</t>
   </si>
   <si>
@@ -245,9 +224,6 @@
     <t xml:space="preserve"> 3.3</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 14</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.05263157894736842</t>
   </si>
   <si>
@@ -269,9 +245,6 @@
     <t xml:space="preserve"> 0.028360962867736816</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 17</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.125</t>
   </si>
   <si>
@@ -305,9 +278,6 @@
     <t xml:space="preserve"> 0.06253194808959961</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 16</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.4666666666666667</t>
   </si>
   <si>
@@ -323,9 +293,6 @@
     <t xml:space="preserve"> 5.7</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 10</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.18181818181818182</t>
   </si>
   <si>
@@ -383,9 +350,6 @@
     <t xml:space="preserve"> 0.06056678295135498</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 11</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.55</t>
   </si>
   <si>
@@ -434,9 +398,6 @@
     <t xml:space="preserve"> 0.046655586787632534</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 36</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.5483870967741935</t>
   </si>
   <si>
@@ -449,9 +410,6 @@
     <t xml:space="preserve"> 0.039666993277413506</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 21</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.52</t>
   </si>
   <si>
@@ -527,9 +485,6 @@
     <t xml:space="preserve"> 5.3</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 23</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.32</t>
   </si>
   <si>
@@ -620,9 +575,6 @@
     <t xml:space="preserve"> 5.25</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 15</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.15547490119934082</t>
   </si>
   <si>
@@ -632,9 +584,6 @@
     <t xml:space="preserve"> 0.05182496706644694</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 22</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.5714285714285714</t>
   </si>
   <si>
@@ -701,9 +650,6 @@
     <t xml:space="preserve"> 7.5</t>
   </si>
   <si>
-    <t>Neighbour got out of range. 19</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.11202645301818848</t>
   </si>
   <si>
@@ -711,6 +657,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 0.03734215100606283</t>
+  </si>
+  <si>
+    <t>Neighbour got out of range.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neighbour got out of range. </t>
   </si>
 </sst>
 </file>
@@ -777,7 +729,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -793,7 +745,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1091,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668B5660-EE48-1D43-A41B-2C53A281025C}">
   <dimension ref="A1:R830"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="F166" sqref="F166"/>
+    <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
+      <selection activeCell="M621" sqref="M621"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1232,12 +1184,17 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>206</v>
+      </c>
+      <c r="B9" s="2">
+        <v>6</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M9" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -1352,13 +1309,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -1372,7 +1329,7 @@
         <v>19</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1380,13 +1337,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -1394,13 +1351,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1408,13 +1365,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L23" t="s">
         <v>22</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -1525,7 +1482,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>29</v>
@@ -1553,13 +1510,13 @@
         <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L34" t="s">
         <v>31</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
@@ -1686,12 +1643,17 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>206</v>
+      </c>
+      <c r="B45" s="2">
+        <v>5</v>
       </c>
       <c r="L45" t="s">
-        <v>36</v>
-      </c>
-      <c r="M45" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M45" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
@@ -1806,13 +1768,13 @@
         <v>17</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -1826,7 +1788,7 @@
         <v>19</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
@@ -1834,13 +1796,13 @@
         <v>20</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -1848,13 +1810,13 @@
         <v>21</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>21</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
@@ -1862,13 +1824,13 @@
         <v>22</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="L59" t="s">
         <v>22</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -2013,7 +1975,7 @@
         <v>31</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
@@ -2140,12 +2102,17 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>62</v>
+        <v>206</v>
+      </c>
+      <c r="B81" s="2">
+        <v>13</v>
       </c>
       <c r="L81" t="s">
-        <v>88</v>
-      </c>
-      <c r="M81" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M81" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M82" s="2"/>
@@ -2256,13 +2223,13 @@
         <v>17</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="L91" t="s">
         <v>17</v>
       </c>
       <c r="M91" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
@@ -2284,13 +2251,13 @@
         <v>20</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="L93" t="s">
         <v>20</v>
       </c>
       <c r="M93" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -2298,13 +2265,13 @@
         <v>21</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="L94" t="s">
         <v>21</v>
       </c>
       <c r="M94" s="2" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
@@ -2312,13 +2279,13 @@
         <v>22</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="L95" t="s">
         <v>22</v>
       </c>
       <c r="M95" s="2" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -2455,13 +2422,13 @@
         <v>31</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L106" t="s">
         <v>31</v>
       </c>
       <c r="M106" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.2">
@@ -2586,12 +2553,17 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>68</v>
+        <v>206</v>
+      </c>
+      <c r="B117" s="2">
+        <v>14</v>
       </c>
       <c r="L117" t="s">
-        <v>114</v>
-      </c>
-      <c r="M117" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M117" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M118" s="2"/>
@@ -2702,13 +2674,13 @@
         <v>17</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="L127" t="s">
         <v>17</v>
       </c>
       <c r="M127" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
@@ -2730,13 +2702,13 @@
         <v>20</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L129" t="s">
         <v>20</v>
       </c>
       <c r="M129" s="2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.2">
@@ -2744,13 +2716,13 @@
         <v>21</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="L130" t="s">
         <v>21</v>
       </c>
       <c r="M130" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.2">
@@ -2758,13 +2730,13 @@
         <v>22</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L131" t="s">
         <v>22</v>
       </c>
       <c r="M131" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.2">
@@ -2901,13 +2873,13 @@
         <v>31</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L142" t="s">
         <v>31</v>
       </c>
       <c r="M142" s="2" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.2">
@@ -3032,12 +3004,17 @@
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>39</v>
+        <v>207</v>
+      </c>
+      <c r="B153" s="2">
+        <v>20</v>
       </c>
       <c r="L153" t="s">
-        <v>162</v>
-      </c>
-      <c r="M153" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M153" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M154" s="2"/>
@@ -3148,13 +3125,13 @@
         <v>17</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="L163" t="s">
         <v>17</v>
       </c>
       <c r="M163" s="2" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.2">
@@ -3176,13 +3153,13 @@
         <v>20</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="L165" t="s">
         <v>20</v>
       </c>
       <c r="M165" s="2" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.2">
@@ -3190,13 +3167,13 @@
         <v>21</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="L166" t="s">
         <v>21</v>
       </c>
       <c r="M166" s="2" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.2">
@@ -3204,13 +3181,13 @@
         <v>22</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="L167" t="s">
         <v>22</v>
       </c>
       <c r="M167" s="2" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.2">
@@ -3347,13 +3324,13 @@
         <v>31</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L178" t="s">
         <v>31</v>
       </c>
       <c r="M178" s="2" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.2">
@@ -3478,12 +3455,17 @@
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>76</v>
+        <v>206</v>
+      </c>
+      <c r="B189" s="2">
+        <v>17</v>
       </c>
       <c r="L189" t="s">
-        <v>162</v>
-      </c>
-      <c r="M189" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M189" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M190" s="2"/>
@@ -3594,13 +3576,13 @@
         <v>17</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="L199" t="s">
         <v>17</v>
       </c>
       <c r="M199" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.2">
@@ -3622,13 +3604,13 @@
         <v>20</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="L201" t="s">
         <v>20</v>
       </c>
       <c r="M201" s="2" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.2">
@@ -3636,13 +3618,13 @@
         <v>21</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="L202" t="s">
         <v>21</v>
       </c>
       <c r="M202" s="2" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.2">
@@ -3650,13 +3632,13 @@
         <v>22</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="L203" t="s">
         <v>22</v>
       </c>
       <c r="M203" s="2" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.2">
@@ -3793,13 +3775,13 @@
         <v>31</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L214" t="s">
         <v>31</v>
       </c>
       <c r="M214" s="2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.2">
@@ -3924,12 +3906,17 @@
     </row>
     <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>44</v>
+        <v>206</v>
+      </c>
+      <c r="B225" s="2">
+        <v>6</v>
       </c>
       <c r="L225" t="s">
-        <v>114</v>
-      </c>
-      <c r="M225" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M225" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M226" s="2"/>
@@ -4040,13 +4027,13 @@
         <v>17</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L235" t="s">
         <v>17</v>
       </c>
       <c r="M235" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.2">
@@ -4054,13 +4041,13 @@
         <v>19</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L236" t="s">
         <v>19</v>
       </c>
       <c r="M236" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="237" spans="1:13" x14ac:dyDescent="0.2">
@@ -4068,13 +4055,13 @@
         <v>20</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L237" t="s">
         <v>20</v>
       </c>
       <c r="M237" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
     </row>
     <row r="238" spans="1:13" x14ac:dyDescent="0.2">
@@ -4082,13 +4069,13 @@
         <v>21</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="L238" t="s">
         <v>21</v>
       </c>
       <c r="M238" s="2" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="239" spans="1:13" x14ac:dyDescent="0.2">
@@ -4096,13 +4083,13 @@
         <v>22</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="L239" t="s">
         <v>22</v>
       </c>
       <c r="M239" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="240" spans="1:13" x14ac:dyDescent="0.2">
@@ -4239,13 +4226,13 @@
         <v>31</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="L250" t="s">
         <v>31</v>
       </c>
       <c r="M250" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="251" spans="1:18" x14ac:dyDescent="0.2">
@@ -4370,12 +4357,17 @@
     </row>
     <row r="261" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>44</v>
+        <v>206</v>
+      </c>
+      <c r="B261" s="2">
+        <v>6</v>
       </c>
       <c r="L261" t="s">
-        <v>94</v>
-      </c>
-      <c r="M261" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M261" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M262" s="2"/>
@@ -4486,13 +4478,13 @@
         <v>17</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L271" t="s">
         <v>17</v>
       </c>
       <c r="M271" s="2" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="272" spans="1:13" x14ac:dyDescent="0.2">
@@ -4500,7 +4492,7 @@
         <v>19</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L272" t="s">
         <v>19</v>
@@ -4514,13 +4506,13 @@
         <v>20</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="L273" t="s">
         <v>20</v>
       </c>
       <c r="M273" s="2" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.2">
@@ -4528,13 +4520,13 @@
         <v>21</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="L274" t="s">
         <v>21</v>
       </c>
       <c r="M274" s="2" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
     </row>
     <row r="275" spans="1:13" x14ac:dyDescent="0.2">
@@ -4542,13 +4534,13 @@
         <v>22</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="L275" t="s">
         <v>22</v>
       </c>
       <c r="M275" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.2">
@@ -4685,13 +4677,13 @@
         <v>31</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="L286" t="s">
         <v>31</v>
       </c>
       <c r="M286" s="2" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
     <row r="287" spans="1:13" x14ac:dyDescent="0.2">
@@ -4816,12 +4808,17 @@
     </row>
     <row r="297" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>88</v>
+        <v>206</v>
+      </c>
+      <c r="B297" s="2">
+        <v>16</v>
       </c>
       <c r="L297" t="s">
-        <v>39</v>
-      </c>
-      <c r="M297" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M297" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="298" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M298" s="2"/>
@@ -4932,13 +4929,13 @@
         <v>17</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="L307" t="s">
         <v>17</v>
       </c>
       <c r="M307" s="2" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="308" spans="1:13" x14ac:dyDescent="0.2">
@@ -4960,13 +4957,13 @@
         <v>20</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="L309" t="s">
         <v>20</v>
       </c>
       <c r="M309" s="2" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
     <row r="310" spans="1:13" x14ac:dyDescent="0.2">
@@ -4974,13 +4971,13 @@
         <v>21</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="L310" t="s">
         <v>21</v>
       </c>
       <c r="M310" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="311" spans="1:13" x14ac:dyDescent="0.2">
@@ -4988,13 +4985,13 @@
         <v>22</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="L311" t="s">
         <v>22</v>
       </c>
       <c r="M311" s="2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.2">
@@ -5131,13 +5128,13 @@
         <v>31</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="L322" t="s">
         <v>31</v>
       </c>
       <c r="M322" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="323" spans="1:18" x14ac:dyDescent="0.2">
@@ -5262,12 +5259,17 @@
     </row>
     <row r="333" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>94</v>
+        <v>206</v>
+      </c>
+      <c r="B333" s="2">
+        <v>10</v>
       </c>
       <c r="L333" t="s">
-        <v>50</v>
-      </c>
-      <c r="M333" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M333" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="334" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M334" s="2"/>
@@ -5378,7 +5380,7 @@
         <v>17</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="L343" t="s">
         <v>17</v>
@@ -5398,7 +5400,7 @@
         <v>19</v>
       </c>
       <c r="M344" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.2">
@@ -5406,13 +5408,13 @@
         <v>20</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="L345" t="s">
         <v>20</v>
       </c>
       <c r="M345" s="2" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
     </row>
     <row r="346" spans="1:13" x14ac:dyDescent="0.2">
@@ -5420,13 +5422,13 @@
         <v>21</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="L346" t="s">
         <v>21</v>
       </c>
       <c r="M346" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
     </row>
     <row r="347" spans="1:13" x14ac:dyDescent="0.2">
@@ -5434,13 +5436,13 @@
         <v>22</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="L347" t="s">
         <v>22</v>
       </c>
       <c r="M347" s="2" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
     </row>
     <row r="348" spans="1:13" x14ac:dyDescent="0.2">
@@ -5577,13 +5579,13 @@
         <v>31</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="L358" t="s">
         <v>31</v>
       </c>
       <c r="M358" s="2" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="359" spans="1:18" x14ac:dyDescent="0.2">
@@ -5708,12 +5710,17 @@
     </row>
     <row r="369" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
-        <v>49</v>
+        <v>206</v>
+      </c>
+      <c r="B369" s="2">
+        <v>33</v>
       </c>
       <c r="L369" t="s">
-        <v>76</v>
-      </c>
-      <c r="M369" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M369" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="370" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M370" s="2"/>
@@ -5824,13 +5831,13 @@
         <v>17</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="L379" t="s">
         <v>17</v>
       </c>
       <c r="M379" s="2" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
     </row>
     <row r="380" spans="1:13" x14ac:dyDescent="0.2">
@@ -5844,7 +5851,7 @@
         <v>19</v>
       </c>
       <c r="M380" s="2" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="381" spans="1:13" x14ac:dyDescent="0.2">
@@ -5852,13 +5859,13 @@
         <v>20</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="L381" t="s">
         <v>20</v>
       </c>
       <c r="M381" s="2" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="382" spans="1:13" x14ac:dyDescent="0.2">
@@ -5866,13 +5873,13 @@
         <v>21</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="L382" t="s">
         <v>21</v>
       </c>
       <c r="M382" s="2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
     </row>
     <row r="383" spans="1:13" x14ac:dyDescent="0.2">
@@ -5880,13 +5887,13 @@
         <v>22</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="L383" t="s">
         <v>22</v>
       </c>
       <c r="M383" s="2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="384" spans="1:13" x14ac:dyDescent="0.2">
@@ -6023,13 +6030,13 @@
         <v>31</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="L394" t="s">
         <v>31</v>
       </c>
       <c r="M394" s="2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="395" spans="1:18" x14ac:dyDescent="0.2">
@@ -6222,18 +6229,22 @@
     </row>
     <row r="405" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A405" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B405" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="B405" s="5">
+        <v>16</v>
+      </c>
       <c r="C405" s="4"/>
       <c r="D405" s="4"/>
       <c r="E405" s="4"/>
       <c r="F405" s="4"/>
       <c r="G405" s="4"/>
       <c r="L405" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="M405" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="M405" s="5">
+        <v>15</v>
+      </c>
       <c r="N405" s="4"/>
       <c r="O405" s="4"/>
       <c r="P405" s="4"/>
@@ -6445,7 +6456,7 @@
         <v>17</v>
       </c>
       <c r="B415" s="5" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C415" s="4"/>
       <c r="D415" s="4"/>
@@ -6456,7 +6467,7 @@
         <v>17</v>
       </c>
       <c r="M415" s="5" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="N415" s="4"/>
       <c r="O415" s="4"/>
@@ -6469,7 +6480,7 @@
         <v>19</v>
       </c>
       <c r="B416" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C416" s="4"/>
       <c r="D416" s="4"/>
@@ -6493,7 +6504,7 @@
         <v>20</v>
       </c>
       <c r="B417" s="5" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C417" s="4"/>
       <c r="D417" s="4"/>
@@ -6504,7 +6515,7 @@
         <v>20</v>
       </c>
       <c r="M417" s="5" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="N417" s="4"/>
       <c r="O417" s="4"/>
@@ -6517,7 +6528,7 @@
         <v>21</v>
       </c>
       <c r="B418" s="5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C418" s="4"/>
       <c r="D418" s="4"/>
@@ -6528,7 +6539,7 @@
         <v>21</v>
       </c>
       <c r="M418" s="5" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="N418" s="4"/>
       <c r="O418" s="4"/>
@@ -6541,7 +6552,7 @@
         <v>22</v>
       </c>
       <c r="B419" s="5" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C419" s="4"/>
       <c r="D419" s="4"/>
@@ -6552,7 +6563,7 @@
         <v>22</v>
       </c>
       <c r="M419" s="5" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="N419" s="4"/>
       <c r="O419" s="4"/>
@@ -6797,7 +6808,7 @@
         <v>31</v>
       </c>
       <c r="B430" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C430" s="4"/>
       <c r="D430" s="4"/>
@@ -6808,7 +6819,7 @@
         <v>31</v>
       </c>
       <c r="M430" s="5" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="N430" s="4"/>
       <c r="O430" s="4"/>
@@ -7042,18 +7053,22 @@
     </row>
     <row r="441" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A441" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B441" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="B441" s="5">
+        <v>10</v>
+      </c>
       <c r="C441" s="4"/>
       <c r="D441" s="4"/>
       <c r="E441" s="4"/>
       <c r="F441" s="4"/>
       <c r="G441" s="4"/>
       <c r="L441" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="M441" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="M441" s="5">
+        <v>22</v>
+      </c>
       <c r="N441" s="4"/>
       <c r="O441" s="4"/>
       <c r="P441" s="4"/>
@@ -7265,7 +7280,7 @@
         <v>17</v>
       </c>
       <c r="B451" s="5" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C451" s="4"/>
       <c r="D451" s="4"/>
@@ -7276,7 +7291,7 @@
         <v>17</v>
       </c>
       <c r="M451" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="N451" s="4"/>
       <c r="O451" s="4"/>
@@ -7300,7 +7315,7 @@
         <v>19</v>
       </c>
       <c r="M452" s="5" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="N452" s="4"/>
       <c r="O452" s="4"/>
@@ -7313,7 +7328,7 @@
         <v>20</v>
       </c>
       <c r="B453" s="5" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C453" s="4"/>
       <c r="D453" s="4"/>
@@ -7324,7 +7339,7 @@
         <v>20</v>
       </c>
       <c r="M453" s="5" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="N453" s="4"/>
       <c r="O453" s="4"/>
@@ -7337,7 +7352,7 @@
         <v>21</v>
       </c>
       <c r="B454" s="5" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C454" s="4"/>
       <c r="D454" s="4"/>
@@ -7348,7 +7363,7 @@
         <v>21</v>
       </c>
       <c r="M454" s="5" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="N454" s="4"/>
       <c r="O454" s="4"/>
@@ -7361,7 +7376,7 @@
         <v>22</v>
       </c>
       <c r="B455" s="5" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C455" s="4"/>
       <c r="D455" s="4"/>
@@ -7372,7 +7387,7 @@
         <v>22</v>
       </c>
       <c r="M455" s="5" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="N455" s="4"/>
       <c r="O455" s="4"/>
@@ -7861,18 +7876,22 @@
     </row>
     <row r="477" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A477" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B477" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="B477" s="5">
+        <v>11</v>
+      </c>
       <c r="C477" s="4"/>
       <c r="D477" s="4"/>
       <c r="E477" s="4"/>
       <c r="F477" s="4"/>
       <c r="G477" s="4"/>
       <c r="L477" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="M477" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="M477" s="5">
+        <v>16</v>
+      </c>
       <c r="N477" s="4"/>
       <c r="O477" s="4"/>
       <c r="P477" s="4"/>
@@ -8084,7 +8103,7 @@
         <v>17</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C487" s="4"/>
       <c r="D487" s="4"/>
@@ -8095,7 +8114,7 @@
         <v>17</v>
       </c>
       <c r="M487" s="5" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="N487" s="4"/>
       <c r="O487" s="4"/>
@@ -8132,7 +8151,7 @@
         <v>20</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C489" s="4"/>
       <c r="D489" s="4"/>
@@ -8143,7 +8162,7 @@
         <v>20</v>
       </c>
       <c r="M489" s="5" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="N489" s="4"/>
       <c r="O489" s="4"/>
@@ -8156,7 +8175,7 @@
         <v>21</v>
       </c>
       <c r="B490" s="5" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C490" s="4"/>
       <c r="D490" s="4"/>
@@ -8167,7 +8186,7 @@
         <v>21</v>
       </c>
       <c r="M490" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="N490" s="4"/>
       <c r="O490" s="4"/>
@@ -8180,7 +8199,7 @@
         <v>22</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C491" s="4"/>
       <c r="D491" s="4"/>
@@ -8191,7 +8210,7 @@
         <v>22</v>
       </c>
       <c r="M491" s="5" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="N491" s="4"/>
       <c r="O491" s="4"/>
@@ -8388,7 +8407,7 @@
         <v>29</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C500" s="4"/>
       <c r="D500" s="4"/>
@@ -8436,7 +8455,7 @@
         <v>31</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C502" s="4"/>
       <c r="D502" s="4"/>
@@ -8681,7 +8700,7 @@
     </row>
     <row r="513" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A513" s="4" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B513" s="5"/>
       <c r="C513" s="4"/>
@@ -8690,7 +8709,7 @@
       <c r="F513" s="4"/>
       <c r="G513" s="4"/>
       <c r="L513" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M513" s="5"/>
       <c r="N513" s="4"/>
@@ -8904,7 +8923,7 @@
         <v>17</v>
       </c>
       <c r="B523" s="5" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C523" s="4"/>
       <c r="D523" s="4"/>
@@ -8915,7 +8934,7 @@
         <v>17</v>
       </c>
       <c r="M523" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="N523" s="4"/>
       <c r="O523" s="4"/>
@@ -8928,7 +8947,7 @@
         <v>19</v>
       </c>
       <c r="B524" s="5" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C524" s="4"/>
       <c r="D524" s="4"/>
@@ -8952,7 +8971,7 @@
         <v>20</v>
       </c>
       <c r="B525" s="5" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C525" s="4"/>
       <c r="D525" s="4"/>
@@ -8963,7 +8982,7 @@
         <v>20</v>
       </c>
       <c r="M525" s="5" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="N525" s="4"/>
       <c r="O525" s="4"/>
@@ -8976,7 +8995,7 @@
         <v>21</v>
       </c>
       <c r="B526" s="5" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C526" s="4"/>
       <c r="D526" s="4"/>
@@ -8987,7 +9006,7 @@
         <v>21</v>
       </c>
       <c r="M526" s="5" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="N526" s="4"/>
       <c r="O526" s="4"/>
@@ -9000,7 +9019,7 @@
         <v>22</v>
       </c>
       <c r="B527" s="5" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C527" s="4"/>
       <c r="D527" s="4"/>
@@ -9011,7 +9030,7 @@
         <v>22</v>
       </c>
       <c r="M527" s="5" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="N527" s="4"/>
       <c r="O527" s="4"/>
@@ -9501,18 +9520,22 @@
     </row>
     <row r="549" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A549" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B549" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="B549" s="5">
+        <v>20</v>
+      </c>
       <c r="C549" s="4"/>
       <c r="D549" s="4"/>
       <c r="E549" s="4"/>
       <c r="F549" s="4"/>
       <c r="G549" s="4"/>
       <c r="L549" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="M549" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="M549" s="5">
+        <v>17</v>
+      </c>
       <c r="N549" s="4"/>
       <c r="O549" s="4"/>
       <c r="P549" s="4"/>
@@ -9724,7 +9747,7 @@
         <v>17</v>
       </c>
       <c r="B559" s="5" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C559" s="4"/>
       <c r="D559" s="4"/>
@@ -9735,7 +9758,7 @@
         <v>17</v>
       </c>
       <c r="M559" s="5" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="N559" s="4"/>
       <c r="O559" s="4"/>
@@ -9759,7 +9782,7 @@
         <v>19</v>
       </c>
       <c r="M560" s="5" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="N560" s="4"/>
       <c r="O560" s="4"/>
@@ -9772,7 +9795,7 @@
         <v>20</v>
       </c>
       <c r="B561" s="5" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C561" s="4"/>
       <c r="D561" s="4"/>
@@ -9783,7 +9806,7 @@
         <v>20</v>
       </c>
       <c r="M561" s="5" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="N561" s="4"/>
       <c r="O561" s="4"/>
@@ -9796,7 +9819,7 @@
         <v>21</v>
       </c>
       <c r="B562" s="5" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C562" s="4"/>
       <c r="D562" s="4"/>
@@ -9807,7 +9830,7 @@
         <v>21</v>
       </c>
       <c r="M562" s="5" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="N562" s="4"/>
       <c r="O562" s="4"/>
@@ -9820,7 +9843,7 @@
         <v>22</v>
       </c>
       <c r="B563" s="5" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C563" s="4"/>
       <c r="D563" s="4"/>
@@ -9831,7 +9854,7 @@
         <v>22</v>
       </c>
       <c r="M563" s="5" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="N563" s="4"/>
       <c r="O563" s="4"/>
@@ -10087,7 +10110,7 @@
         <v>31</v>
       </c>
       <c r="M574" s="5" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="N574" s="4"/>
       <c r="O574" s="4"/>
@@ -10321,18 +10344,22 @@
     </row>
     <row r="585" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A585" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B585" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="B585" s="5">
+        <v>36</v>
+      </c>
       <c r="C585" s="4"/>
       <c r="D585" s="4"/>
       <c r="E585" s="4"/>
       <c r="F585" s="4"/>
       <c r="G585" s="4"/>
       <c r="L585" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="M585" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="M585" s="5">
+        <v>36</v>
+      </c>
       <c r="N585" s="4"/>
       <c r="O585" s="4"/>
       <c r="P585" s="4"/>
@@ -10544,7 +10571,7 @@
         <v>17</v>
       </c>
       <c r="B595" s="5" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C595" s="4"/>
       <c r="D595" s="4"/>
@@ -10555,7 +10582,7 @@
         <v>17</v>
       </c>
       <c r="M595" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="N595" s="4"/>
       <c r="O595" s="4"/>
@@ -10579,7 +10606,7 @@
         <v>19</v>
       </c>
       <c r="M596" s="5" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="N596" s="4"/>
       <c r="O596" s="4"/>
@@ -10592,7 +10619,7 @@
         <v>20</v>
       </c>
       <c r="B597" s="5" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C597" s="4"/>
       <c r="D597" s="4"/>
@@ -10603,7 +10630,7 @@
         <v>20</v>
       </c>
       <c r="M597" s="5" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="N597" s="4"/>
       <c r="O597" s="4"/>
@@ -10616,7 +10643,7 @@
         <v>21</v>
       </c>
       <c r="B598" s="5" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C598" s="4"/>
       <c r="D598" s="4"/>
@@ -10627,7 +10654,7 @@
         <v>21</v>
       </c>
       <c r="M598" s="5" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="N598" s="4"/>
       <c r="O598" s="4"/>
@@ -10640,7 +10667,7 @@
         <v>22</v>
       </c>
       <c r="B599" s="5" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C599" s="4"/>
       <c r="D599" s="4"/>
@@ -10651,7 +10678,7 @@
         <v>22</v>
       </c>
       <c r="M599" s="5" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="N599" s="4"/>
       <c r="O599" s="4"/>
@@ -10907,7 +10934,7 @@
         <v>31</v>
       </c>
       <c r="M610" s="5" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="N610" s="4"/>
       <c r="O610" s="4"/>
@@ -11141,18 +11168,22 @@
     </row>
     <row r="621" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A621" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B621" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="B621" s="5">
+        <v>21</v>
+      </c>
       <c r="C621" s="4"/>
       <c r="D621" s="4"/>
       <c r="E621" s="4"/>
       <c r="F621" s="4"/>
       <c r="G621" s="4"/>
       <c r="L621" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="M621" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="M621" s="5">
+        <v>19</v>
+      </c>
       <c r="N621" s="4"/>
       <c r="O621" s="4"/>
       <c r="P621" s="4"/>
@@ -11364,7 +11395,7 @@
         <v>17</v>
       </c>
       <c r="B631" s="5" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C631" s="4"/>
       <c r="D631" s="4"/>
@@ -11375,7 +11406,7 @@
         <v>17</v>
       </c>
       <c r="M631" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="N631" s="4"/>
       <c r="O631" s="4"/>
@@ -11412,7 +11443,7 @@
         <v>20</v>
       </c>
       <c r="B633" s="5" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C633" s="4"/>
       <c r="D633" s="4"/>
@@ -11423,7 +11454,7 @@
         <v>20</v>
       </c>
       <c r="M633" s="5" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="N633" s="4"/>
       <c r="O633" s="4"/>
@@ -11436,7 +11467,7 @@
         <v>21</v>
       </c>
       <c r="B634" s="5" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C634" s="4"/>
       <c r="D634" s="4"/>
@@ -11447,7 +11478,7 @@
         <v>21</v>
       </c>
       <c r="M634" s="5" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="N634" s="4"/>
       <c r="O634" s="4"/>
@@ -11460,7 +11491,7 @@
         <v>22</v>
       </c>
       <c r="B635" s="5" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C635" s="4"/>
       <c r="D635" s="4"/>
@@ -11471,7 +11502,7 @@
         <v>22</v>
       </c>
       <c r="M635" s="5" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="N635" s="4"/>
       <c r="O635" s="4"/>
@@ -11727,7 +11758,7 @@
         <v>31</v>
       </c>
       <c r="M646" s="5" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="N646" s="4"/>
       <c r="O646" s="4"/>

</xml_diff>